<commit_message>
Cambios en el base_datos_app
</commit_message>
<xml_diff>
--- a/folder_test/formato_estandar_po_cotizacion.xlsx
+++ b/folder_test/formato_estandar_po_cotizacion.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\OneDrive\Escritorio\idm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C5CE2D-F901-4864-98BC-697B433CABEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F065200-594A-4E05-99F5-CB6EA02D888A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16860" xr2:uid="{2FC6E42C-2136-4FEA-9A66-F3C3317047E6}"/>
   </bookViews>
   <sheets>
-    <sheet name="cotizacion " sheetId="5" r:id="rId1"/>
+    <sheet name="cotizacion" sheetId="5" r:id="rId1"/>
     <sheet name="po" sheetId="1" r:id="rId2"/>
     <sheet name="datos_de_cliente" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'cotizacion '!$A$1:$I$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">cotizacion!$A$1:$I$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">po!$A$1:$I$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1303,221 +1303,221 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1979,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674D57B5-3031-4762-9614-4044D8E8AF41}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:I3"/>
     </sheetView>
   </sheetViews>
@@ -1999,39 +1999,39 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="67"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="2"/>
       <c r="E2" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="F2" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="2"/>
       <c r="E3" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="88" t="str">
+      <c r="F3" s="66" t="str">
         <f>VLOOKUP(F2, datos_de_cliente!D:E, 2, FALSE)</f>
         <v>GUTA540927QW6</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
     </row>
     <row r="4" spans="1:14" ht="20.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:14" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2041,21 +2041,21 @@
       <c r="B5" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="129"/>
-      <c r="E5" s="128" t="s">
+      <c r="D5" s="68"/>
+      <c r="E5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="130"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="131" t="s">
+      <c r="H5" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="132"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:14" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
@@ -2064,20 +2064,20 @@
       <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="61" t="str">
+      <c r="D6" s="73"/>
+      <c r="E6" s="74" t="str">
         <f>VLOOKUP(C6, datos_de_cliente!A:B, 2, FALSE)</f>
         <v>C. 5 Nte. 511, Centenario, Cd Industrial, 22444 Tijuana, B.C.</v>
       </c>
-      <c r="F6" s="62"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="65" t="s">
+      <c r="H6" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="66"/>
+      <c r="I6" s="77"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2086,44 +2086,44 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="41"/>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="126"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" spans="1:14" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="16" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="91" t="s">
+      <c r="H8" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="91"/>
+      <c r="I8" s="93"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="127" t="s">
+      <c r="A9" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="127"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="58">
         <v>1</v>
       </c>
@@ -2139,13 +2139,13 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
@@ -2162,13 +2162,13 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="6">
         <v>3</v>
       </c>
@@ -2185,13 +2185,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="50">
         <v>4</v>
       </c>
@@ -2208,13 +2208,13 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
       <c r="F13" s="6">
         <v>5</v>
       </c>
@@ -2231,13 +2231,13 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
       <c r="F14" s="6">
         <v>6</v>
       </c>
@@ -2254,13 +2254,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
       <c r="F15" s="6">
         <v>7</v>
       </c>
@@ -2277,11 +2277,11 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="80"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
       <c r="F16" s="6"/>
       <c r="G16" s="43"/>
       <c r="H16" s="49">
@@ -2294,11 +2294,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
       <c r="F17" s="6"/>
       <c r="G17" s="43"/>
       <c r="H17" s="49">
@@ -2311,11 +2311,11 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="6"/>
       <c r="G18" s="43"/>
       <c r="H18" s="49">
@@ -2328,11 +2328,11 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="6"/>
       <c r="G19" s="43"/>
       <c r="H19" s="49">
@@ -2345,11 +2345,11 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
       <c r="F20" s="6"/>
       <c r="G20" s="43"/>
       <c r="H20" s="49">
@@ -2362,11 +2362,11 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
+      <c r="A21" s="81"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="6"/>
       <c r="G21" s="43"/>
       <c r="H21" s="49">
@@ -2379,11 +2379,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
       <c r="F22" s="6"/>
       <c r="G22" s="43"/>
       <c r="H22" s="49">
@@ -2396,11 +2396,11 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="80"/>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
       <c r="F23" s="6"/>
       <c r="G23" s="43"/>
       <c r="H23" s="49">
@@ -2413,11 +2413,11 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
       <c r="F24" s="6"/>
       <c r="G24" s="43"/>
       <c r="H24" s="49">
@@ -2430,11 +2430,11 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="80"/>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
       <c r="F25" s="6"/>
       <c r="G25" s="43"/>
       <c r="H25" s="49">
@@ -2447,11 +2447,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
       <c r="F26" s="6"/>
       <c r="G26" s="43"/>
       <c r="H26" s="49">
@@ -2464,11 +2464,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="80"/>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
       <c r="F27" s="6"/>
       <c r="G27" s="43"/>
       <c r="H27" s="49">
@@ -2481,11 +2481,11 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="80"/>
-      <c r="B28" s="80"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
       <c r="F28" s="6"/>
       <c r="G28" s="43"/>
       <c r="H28" s="49">
@@ -2498,11 +2498,11 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="80"/>
-      <c r="B29" s="80"/>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
+      <c r="A29" s="81"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
       <c r="F29" s="6"/>
       <c r="G29" s="43"/>
       <c r="H29" s="49">
@@ -2515,11 +2515,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="80"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
       <c r="F30" s="6"/>
       <c r="G30" s="43"/>
       <c r="H30" s="49">
@@ -2532,11 +2532,11 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="80"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
+      <c r="A31" s="81"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
       <c r="F31" s="6"/>
       <c r="G31" s="43"/>
       <c r="H31" s="49">
@@ -2549,11 +2549,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="90"/>
-      <c r="B32" s="90"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
+      <c r="A32" s="114"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
       <c r="F32" s="22"/>
       <c r="G32" s="44"/>
       <c r="H32" s="49">
@@ -2566,119 +2566,119 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="110" t="s">
+      <c r="A33" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="111"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="118"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="85"/>
       <c r="F33" s="38"/>
-      <c r="G33" s="98" t="s">
+      <c r="G33" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="100">
+      <c r="H33" s="102">
         <f>SUM(H9:H31)</f>
         <v>140</v>
       </c>
-      <c r="I33" s="101"/>
+      <c r="I33" s="103"/>
     </row>
     <row r="34" spans="1:9" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="112"/>
-      <c r="B34" s="113"/>
-      <c r="C34" s="119"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="120"/>
+      <c r="A34" s="117"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="88"/>
       <c r="F34" s="35"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="102"/>
+      <c r="G34" s="100"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="105"/>
     </row>
     <row r="35" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="114"/>
-      <c r="B35" s="115"/>
-      <c r="C35" s="121"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="123"/>
+      <c r="A35" s="119"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="91"/>
       <c r="F35" s="36"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="104"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="107"/>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="92" t="s">
+      <c r="A36" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="92"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="93"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="95"/>
       <c r="G36" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="105">
+      <c r="H36" s="108">
         <f>H33*0.16</f>
         <v>22.400000000000002</v>
       </c>
-      <c r="I36" s="106"/>
+      <c r="I36" s="109"/>
     </row>
     <row r="37" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
       <c r="D37" s="37"/>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="97"/>
+      <c r="F37" s="99"/>
       <c r="G37" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="107">
+      <c r="H37" s="110">
         <f>H33+H36</f>
         <v>162.4</v>
       </c>
-      <c r="I37" s="108"/>
+      <c r="I37" s="111"/>
     </row>
     <row r="38" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="109" t="s">
+      <c r="A38" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="109"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="109"/>
-      <c r="F38" s="109"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
     </row>
     <row r="39" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="74"/>
-      <c r="B39" s="74"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="113"/>
+      <c r="E39" s="113"/>
+      <c r="F39" s="113"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="113"/>
+      <c r="I39" s="113"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="83" t="s">
+      <c r="A40" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="83"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="92"/>
+      <c r="I40" s="92"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I41" s="30"/>
@@ -2686,38 +2686,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="48">
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="C33:E35"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
     <mergeCell ref="A40:I40"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A36:F36"/>
@@ -2734,6 +2702,38 @@
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A33:B35"/>
+    <mergeCell ref="C33:E35"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9" xr:uid="{42CB4AA1-3A39-45D0-B4FE-2078893F2A5B}">
@@ -2793,37 +2793,37 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="67"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="F2" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="88" t="str">
+      <c r="E3" s="63"/>
+      <c r="F3" s="66" t="str">
         <f>VLOOKUP(F2, datos_de_cliente!D:E, 2, FALSE)</f>
         <v>CUTA580917281</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
     </row>
     <row r="4" spans="1:14" ht="20.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:14" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2833,21 +2833,21 @@
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="84" t="s">
+      <c r="D5" s="123"/>
+      <c r="E5" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="85"/>
+      <c r="F5" s="122"/>
       <c r="G5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="84" t="s">
+      <c r="H5" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="85"/>
+      <c r="I5" s="122"/>
     </row>
     <row r="6" spans="1:14" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
@@ -2856,22 +2856,22 @@
       <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="61" t="str">
+      <c r="D6" s="73"/>
+      <c r="E6" s="74" t="str">
         <f>VLOOKUP(C6, datos_de_cliente!A:B, 2, FALSE)</f>
         <v>Paseo del Cucapah 10510 El Lago, Lago Sur, 22210 B.C.</v>
       </c>
-      <c r="F6" s="62"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="65" t="s">
+      <c r="H6" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="66"/>
+      <c r="I6" s="77"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2880,25 +2880,25 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
     </row>
     <row r="8" spans="1:14" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="16" t="s">
         <v>17</v>
       </c>
@@ -2913,13 +2913,13 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
       <c r="F9">
         <v>1</v>
       </c>
@@ -2935,13 +2935,13 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
       <c r="F10" s="6">
         <v>2</v>
       </c>
@@ -2958,13 +2958,13 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="6">
         <v>3</v>
       </c>
@@ -2981,13 +2981,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="6">
         <v>4</v>
       </c>
@@ -3004,13 +3004,13 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
       <c r="F13" s="6">
         <v>5</v>
       </c>
@@ -3027,13 +3027,13 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
       <c r="F14" s="6">
         <v>6</v>
       </c>
@@ -3050,13 +3050,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
       <c r="F15" s="6">
         <v>7</v>
       </c>
@@ -3073,11 +3073,11 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="80"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7">
@@ -3090,11 +3090,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7">
@@ -3107,11 +3107,11 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7">
@@ -3124,11 +3124,11 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7">
@@ -3141,11 +3141,11 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7">
@@ -3158,11 +3158,11 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
+      <c r="A21" s="81"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
@@ -3175,11 +3175,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
       <c r="F22" s="6"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
@@ -3192,11 +3192,11 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="80"/>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
@@ -3209,11 +3209,11 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7">
@@ -3226,11 +3226,11 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="80"/>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
       <c r="F25" s="6"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7">
@@ -3243,11 +3243,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
       <c r="F26" s="6"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7">
@@ -3260,11 +3260,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="80"/>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
       <c r="F27" s="6"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7">
@@ -3277,11 +3277,11 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="80"/>
-      <c r="B28" s="80"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7">
@@ -3294,11 +3294,11 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="80"/>
-      <c r="B29" s="80"/>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
+      <c r="A29" s="81"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7">
@@ -3311,11 +3311,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="80"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7">
@@ -3328,11 +3328,11 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="80"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
+      <c r="A31" s="81"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
       <c r="F31" s="6"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7">
@@ -3345,11 +3345,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="90"/>
-      <c r="B32" s="90"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
+      <c r="A32" s="114"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
       <c r="F32" s="6"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21">
@@ -3362,43 +3362,43 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="79" t="s">
+      <c r="G33" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="78">
+      <c r="H33" s="104">
         <f>SUM(H9:H31)</f>
         <v>140</v>
       </c>
-      <c r="I33" s="78"/>
+      <c r="I33" s="104"/>
     </row>
     <row r="34" spans="1:9" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
+      <c r="A34" s="131"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
+      <c r="G34" s="132"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
     </row>
     <row r="35" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="G35" s="132"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
@@ -3409,67 +3409,97 @@
       <c r="G36" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="70">
+      <c r="H36" s="126">
         <f>H33*0.16</f>
         <v>22.400000000000002</v>
       </c>
-      <c r="I36" s="71"/>
+      <c r="I36" s="127"/>
     </row>
     <row r="37" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="75"/>
-      <c r="B37" s="75"/>
+      <c r="A37" s="130"/>
+      <c r="B37" s="130"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="72">
+      <c r="H37" s="128">
         <f>H33+H36</f>
         <v>162.4</v>
       </c>
-      <c r="I37" s="73"/>
+      <c r="I37" s="129"/>
     </row>
     <row r="38" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="74" t="s">
+      <c r="A38" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="74"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
+      <c r="B38" s="113"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
     </row>
     <row r="39" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="74"/>
-      <c r="B39" s="74"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="113"/>
+      <c r="E39" s="113"/>
+      <c r="F39" s="113"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="113"/>
+      <c r="I39" s="113"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="83" t="s">
+      <c r="A40" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="83"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="92"/>
+      <c r="I40" s="92"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="46">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A38:I39"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C33:E35"/>
+    <mergeCell ref="A33:B35"/>
+    <mergeCell ref="H33:I35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
     <mergeCell ref="A40:I40"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="E5:F5"/>
@@ -3486,36 +3516,6 @@
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="A38:I39"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C33:E35"/>
-    <mergeCell ref="A33:B35"/>
-    <mergeCell ref="H33:I35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9" xr:uid="{539EE2B9-C8CA-4C31-B136-026A2BAF6DC9}">

</xml_diff>